<commit_message>
plot updates and poster
</commit_message>
<xml_diff>
--- a/GUA work/Pt(100)/IR chamber/GUA 0.025 L.xlsx
+++ b/GUA work/Pt(100)/IR chamber/GUA 0.025 L.xlsx
@@ -9067,7 +9067,7 @@
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>QMS signal</a:t>
+                  <a:t>QMS Intensity</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -22300,74 +22300,6 @@
       </cdr:txBody>
     </cdr:sp>
   </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.76212</cdr:x>
-      <cdr:y>0.06152</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.88712</cdr:x>
-      <cdr:y>0.13424</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="10" name="TextBox 9">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D654D679-C0EB-44E4-9256-29FE1C1300AF}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5575070" y="281249"/>
-          <a:ext cx="914400" cy="332509"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" b="0" i="0" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>GUA/Pt(100)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1600">
-            <a:effectLst/>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
 </c:userShapes>
 </file>
 
@@ -51713,7 +51645,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>